<commit_message>
modified:   final.xlsx 	new file:   homeworkchecker v2.5.py
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -360,7 +360,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C1" t="inlineStr">
         <is>
@@ -377,7 +377,32 @@
           <t>A</t>
         </is>
       </c>
-      <c r="F1" t="n">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -388,7 +413,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -405,8 +430,33 @@
           <t>B</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>10</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -416,7 +466,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -433,7 +483,32 @@
           <t>C</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
         <v>20</v>
       </c>
     </row>
@@ -444,24 +519,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
+          <t>E</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>